<commit_message>
deleting issue #9.0: adesso il codice funziona. Prima il replace inseriva // invece che / nel path dei file quindi l'algoritmo non riusciva a trovare i matching tra i file dei commit e quelli delle release
</commit_message>
<xml_diff>
--- a/bookkeeper-report.xlsx
+++ b/bookkeeper-report.xlsx
@@ -38,7 +38,7 @@
     <t>Bookkeeper</t>
   </si>
   <si>
-    <t>1, 4.1.0</t>
+    <t>, 4.0.0</t>
   </si>
   <si>
     <t>Naive Bayes</t>
@@ -50,7 +50,7 @@
     <t>0.02702702702702703</t>
   </si>
   <si>
-    <t>0.3088803088803089</t>
+    <t>0.29120879120879123</t>
   </si>
   <si>
     <t>-0.20673172674766</t>
@@ -71,46 +71,43 @@
     <t>IBk</t>
   </si>
   <si>
-    <t>2, 4.2.0</t>
-  </si>
-  <si>
-    <t>0.3333333333333333</t>
-  </si>
-  <si>
-    <t>0.22727272727272727</t>
-  </si>
-  <si>
-    <t>0.671907040328093</t>
-  </si>
-  <si>
-    <t>0.175369458128079</t>
+    <t>, 4.0.0, 4.1.0</t>
+  </si>
+  <si>
+    <t>0.35294117647058826</t>
+  </si>
+  <si>
+    <t>0.2727272727272727</t>
+  </si>
+  <si>
+    <t>0.689935064935065</t>
+  </si>
+  <si>
+    <t>0.20993014914102326</t>
+  </si>
+  <si>
+    <t>0.6883116883116883</t>
+  </si>
+  <si>
+    <t>0.25</t>
   </si>
   <si>
     <t>0.045454545454545456</t>
   </si>
   <si>
-    <t>0.6455058099794941</t>
-  </si>
-  <si>
-    <t>0.04755543681538863</t>
-  </si>
-  <si>
-    <t>0.06818181818181818</t>
-  </si>
-  <si>
-    <t>0.5826640464798359</t>
-  </si>
-  <si>
-    <t>0.08896606999732835</t>
-  </si>
-  <si>
-    <t>3, 4.2.1</t>
-  </si>
-  <si>
-    <t>0.8028879015721121</t>
-  </si>
-  <si>
-    <t>0.5893284347231715</t>
+    <t>0.5673701298701299</t>
+  </si>
+  <si>
+    <t>0.03476907109496633</t>
+  </si>
+  <si>
+    <t>, 4.0.0, 4.1.0, 4.2.0</t>
+  </si>
+  <si>
+    <t>0.8030587833219412</t>
+  </si>
+  <si>
+    <t>0.5658749145591251</t>
   </si>
   <si>
     <t>-0.012496449872196011</t>
@@ -122,22 +119,25 @@
     <t>-0.018453795610233626</t>
   </si>
   <si>
-    <t>4, 4.2.2</t>
-  </si>
-  <si>
-    <t>0.8512735127351273</t>
-  </si>
-  <si>
-    <t>0.6786967869678697</t>
-  </si>
-  <si>
-    <t>0.0975609756097561</t>
-  </si>
-  <si>
-    <t>0.8077580775807758</t>
-  </si>
-  <si>
-    <t>0.12575177692728315</t>
+    <t>, 4.0.0, 4.1.0, 4.2.0, 4.2.1</t>
+  </si>
+  <si>
+    <t>0.8496534965349654</t>
+  </si>
+  <si>
+    <t>0.7145171451714517</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.07317073170731707</t>
+  </si>
+  <si>
+    <t>0.8068130681306813</t>
+  </si>
+  <si>
+    <t>0.10486300387318909</t>
   </si>
 </sst>
 </file>
@@ -314,16 +314,16 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
@@ -337,16 +337,16 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8">
@@ -354,7 +354,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -366,7 +366,7 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
@@ -377,7 +377,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -389,10 +389,10 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
         <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -400,7 +400,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -412,10 +412,10 @@
         <v>16</v>
       </c>
       <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
         <v>34</v>
-      </c>
-      <c r="G10" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -423,7 +423,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -435,7 +435,7 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
@@ -446,7 +446,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -458,7 +458,7 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
@@ -469,13 +469,13 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>

</xml_diff>